<commit_message>
added source file for adiw1235-1
</commit_message>
<xml_diff>
--- a/raw/xlsx/numerals-adiw1235-1.xlsx
+++ b/raw/xlsx/numerals-adiw1235-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bibiko/Documents/Developments/shh_git/numeralbank/numerals/raw/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3B4876-002F-9241-BF46-F59F3A5E7185}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC98A298-8A1A-8647-B345-F709FA899849}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="520" yWindow="460" windowWidth="28280" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>NUMERAL</t>
   </si>
@@ -300,6 +300,9 @@
   </si>
   <si>
     <t>Adiwasi Garasia has a native vigesimal numeral system with interesting construction on compound numbers 15 to 19, 26 to 29 and 70 and 90. Second forms of numbers 11 to 19 are borrowed terms used by the literate.</t>
+  </si>
+  <si>
+    <t>Garasia-Adiwasi.htm</t>
   </si>
 </sst>
 </file>
@@ -677,7 +680,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -1288,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1330,11 +1333,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="31" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="6" spans="1:2" ht="31" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">

</xml_diff>